<commit_message>
Put back Meta category for review
</commit_message>
<xml_diff>
--- a/brise_plandok/review/input/review_template.xlsx
+++ b/brise_plandok/review/input/review_template.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Label" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="Attribute" vbProcedure="false">Label!$B$1:$B$14</definedName>
+    <definedName function="false" hidden="false" name="Attribute" vbProcedure="false">Label!$B$1:$B$15</definedName>
     <definedName function="false" hidden="false" name="Attribute_Review" vbProcedure="false">Label!$X$4:$X$6</definedName>
     <definedName function="false" hidden="false" name="Ausgestaltung_und_Sonstiges" vbProcedure="false">Label!$P$4:$P$24</definedName>
     <definedName function="false" hidden="false" name="Dach" vbProcedure="false">Label!$Q$4:$Q$12</definedName>
@@ -23,7 +23,8 @@
     <definedName function="false" hidden="false" name="Hoehe" vbProcedure="false">Label!$H$4:$H$12</definedName>
     <definedName function="false" hidden="false" name="Lage_Gelaende_Planzeichen" vbProcedure="false">Label!$S$4:$S$11</definedName>
     <definedName function="false" hidden="false" name="Laubengaenge_Durchfahrten_Arkaden" vbProcedure="false">Label!$O$4:$O$11</definedName>
-    <definedName function="false" hidden="false" name="Nutzung_Widmung" vbProcedure="false">Label!$M$4:$M$10</definedName>
+    <definedName function="false" hidden="false" name="Meta" vbProcedure="false">Label!$T$4</definedName>
+    <definedName function="false" hidden="false" name="Nutzung_Widmung" vbProcedure="false">Label!$T$7</definedName>
     <definedName function="false" hidden="false" name="Sentence_Review" vbProcedure="false">Label!$Z$4:$Z$5</definedName>
     <definedName function="false" hidden="false" name="Stellplaetze_Garagen_Parkgebäude" vbProcedure="false">Label!$I$4:$I$15</definedName>
     <definedName function="false" hidden="false" name="Strassen_und_Gehsteige" vbProcedure="false">Label!$R$4:$R$8</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="128">
   <si>
     <t xml:space="preserve">Sentence_ID</t>
   </si>
@@ -105,6 +106,9 @@
     <t xml:space="preserve">Lage_Gelaende_Planzeichen</t>
   </si>
   <si>
+    <t xml:space="preserve">Meta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Attribute Review</t>
   </si>
   <si>
@@ -151,6 +155,9 @@
   </si>
   <si>
     <t xml:space="preserve">AnFluchtlinie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error</t>
   </si>
   <si>
     <t xml:space="preserve">OK</t>
@@ -1394,11 +1401,11 @@
   </sheetPr>
   <dimension ref="B1:Z24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O21" activeCellId="0" sqref="O21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T7" activeCellId="0" sqref="T7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.55"/>
@@ -1479,13 +1486,15 @@
       <c r="S3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="T3" s="8"/>
+      <c r="T3" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="U3" s="8"/>
       <c r="X3" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Z3" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,52 +1502,55 @@
         <v>11</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>38</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1546,46 +1558,46 @@
         <v>14</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="X5" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1593,43 +1605,43 @@
         <v>17</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1637,34 +1649,34 @@
         <v>12</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1672,34 +1684,34 @@
         <v>20</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1707,28 +1719,28 @@
         <v>18</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1736,25 +1748,25 @@
         <v>16</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,22 +1774,22 @@
         <v>13</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1785,13 +1797,13 @@
         <v>19</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1799,13 +1811,13 @@
         <v>10</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,63 +1825,67 @@
         <v>15</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="I15" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="8"/>
       <c r="P16" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P17" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P18" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P19" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P20" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P21" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P22" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P23" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P24" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Nuzung_Widmung named range
</commit_message>
<xml_diff>
--- a/brise_plandok/review/input/review_template.xlsx
+++ b/brise_plandok/review/input/review_template.xlsx
@@ -24,7 +24,7 @@
     <definedName function="false" hidden="false" name="Lage_Gelaende_Planzeichen" vbProcedure="false">Label!$S$4:$S$11</definedName>
     <definedName function="false" hidden="false" name="Laubengaenge_Durchfahrten_Arkaden" vbProcedure="false">Label!$O$4:$O$11</definedName>
     <definedName function="false" hidden="false" name="Meta" vbProcedure="false">Label!$T$4</definedName>
-    <definedName function="false" hidden="false" name="Nutzung_Widmung" vbProcedure="false">Label!$T$7</definedName>
+    <definedName function="false" hidden="false" name="Nutzung_Widmung" vbProcedure="false">Label!$M$4:$M$10</definedName>
     <definedName function="false" hidden="false" name="Sentence_Review" vbProcedure="false">Label!$Z$4:$Z$5</definedName>
     <definedName function="false" hidden="false" name="Stellplaetze_Garagen_Parkgebäude" vbProcedure="false">Label!$I$4:$I$15</definedName>
     <definedName function="false" hidden="false" name="Strassen_und_Gehsteige" vbProcedure="false">Label!$R$4:$R$8</definedName>
@@ -1401,11 +1401,11 @@
   </sheetPr>
   <dimension ref="B1:Z24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T7" activeCellId="0" sqref="T7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.55"/>

</xml_diff>

<commit_message>
Color rule-based attributes to gray in review excel
</commit_message>
<xml_diff>
--- a/brise_plandok/review/input/review_template.xlsx
+++ b/brise_plandok/review/input/review_template.xlsx
@@ -719,7 +719,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BP345"/>
+  <dimension ref="A1:BP5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -729,7 +729,7 @@
       <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="64.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.63"/>
@@ -789,7 +789,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="69" style="1" width="8.74"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="6" customFormat="true" ht="64.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -995,10 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="64.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="H5" s="7"/>
       <c r="M5" s="7"/>
       <c r="R5" s="7"/>
@@ -1013,346 +1010,6 @@
       <c r="BK5" s="7"/>
       <c r="BP5" s="7"/>
     </row>
-    <row r="6" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="92" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="100" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="102" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="103" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="104" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="105" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="106" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="107" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="108" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="109" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="110" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="111" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="112" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="113" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="114" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="115" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="116" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="117" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="118" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="119" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="120" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="121" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="122" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="123" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="124" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="125" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="126" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="127" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="128" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="129" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="130" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="131" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="132" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="133" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="134" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="135" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="136" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="137" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="138" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="139" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="140" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="141" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="142" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="143" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="144" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="145" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="146" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="147" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="148" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="149" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="150" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="151" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="152" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="153" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="155" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="156" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="157" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="158" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="159" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="160" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="161" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="162" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="163" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="164" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="165" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="166" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="167" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="168" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="169" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="170" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="171" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="172" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="173" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="174" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="175" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="176" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="177" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="178" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="179" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="180" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="181" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="182" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="183" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="184" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="185" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="186" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="187" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="188" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="189" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="190" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="191" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="192" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="193" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="194" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="195" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="196" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="197" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="198" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="199" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="200" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="201" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="202" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="203" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="204" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="205" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="206" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="207" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="208" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="209" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="210" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="211" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="212" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="213" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="215" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="216" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="219" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="220" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="221" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="222" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="223" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="224" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="225" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="226" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="227" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="228" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="229" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="230" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="231" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="232" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="233" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="234" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="235" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="236" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="237" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="238" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="239" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="240" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="241" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="242" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="243" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="244" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="245" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="246" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="247" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="248" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="249" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="250" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="251" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="252" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="253" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="254" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="255" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="256" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="257" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="258" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="259" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="260" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="261" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="262" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="263" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="264" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="265" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="266" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="267" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="268" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="269" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="270" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="271" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="272" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="273" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="274" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="275" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="276" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="277" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="278" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="279" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="280" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="281" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="282" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="283" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="284" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="285" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="286" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="287" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="288" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="289" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="290" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="291" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="292" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="293" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="294" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="295" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="296" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="297" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="298" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="299" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="300" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="301" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="302" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="303" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="304" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="305" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="306" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="307" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="308" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="309" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="310" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="311" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="312" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="313" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="314" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="315" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="316" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="317" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="318" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="319" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="320" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="321" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="322" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="323" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="324" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="325" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="326" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="327" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="328" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="329" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="330" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="331" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="332" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="333" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="334" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="335" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="336" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="337" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="338" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="339" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="340" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="341" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="342" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="343" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="344" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="345" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="H1:H1048576 M1:M1048576 R1:R1048576 W1:W1048576 AB1:AB1048576 AG1:AG1048576 AL1:AL1048576 AQ1:AQ1048576 AV1:AV1048576 BA1:BA1048576 BF1:BF1048576 BK1:BK1048576 BP1:BP1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
@@ -1405,7 +1062,7 @@
       <selection pane="topLeft" activeCell="T7" activeCellId="0" sqref="T7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.55"/>

</xml_diff>